<commit_message>
fixed a silly error with covars on post-spawning ricker
</commit_message>
<xml_diff>
--- a/data/in/futR_Inputs.xlsx
+++ b/data/in/futR_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LaCie/GitHub_cloud/futR/data/in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E15F9BD-7B11-864C-A0ED-8D35F61DB57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD6A70F-B3CB-9D4C-A9D6-6DCF0993315D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="1880" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10580" yWindow="2220" windowWidth="27640" windowHeight="16940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="switches" sheetId="3" r:id="rId1"/>
@@ -73,7 +73,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -83,7 +83,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Should the model estimate this parameter? 
 </t>
@@ -171,9 +171,6 @@
     <t>estimate</t>
   </si>
   <si>
-    <t>startVal</t>
-  </si>
-  <si>
     <t>Switch</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>rec_year</t>
+  </si>
+  <si>
+    <t>startVal(DEFUNCT)</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1134,15 +1134,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>1E-4</v>
@@ -1184,7 +1184,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1199,7 +1199,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2020,7 +2020,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="str">
         <f>IF(covar_val!B1&lt;&gt;"",covar_val!B1,"NA")</f>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2082,7 +2082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3786,8 +3786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3799,7 +3799,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -3808,7 +3808,7 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>